<commit_message>
achei q tinha ido mas n foi pqp
</commit_message>
<xml_diff>
--- a/Contatos.xlsx
+++ b/Contatos.xlsx
@@ -5,16 +5,21 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MEU COMPUTADOR\OneDrive\Área de Trabalho\SMG\Envio de mensagens\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MEU COMPUTADOR\OneDrive\Área de Trabalho\SMG\robo de mensagens\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34BDFF10-D885-455A-A6F0-4DB7D53C3728}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F289448-621E-46E4-9E5A-7DC159510FAD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="Mensagem">Plan1!$C:$C</definedName>
+    <definedName name="Nome">Plan1!$A:$A</definedName>
+    <definedName name="Número">Plan1!$B:$B</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -354,15 +359,15 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.6796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -373,7 +378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
aparentemente n precisa usar a porra do edge, isso é bom pq eu odeio ele : )
</commit_message>
<xml_diff>
--- a/Contatos.xlsx
+++ b/Contatos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MEU COMPUTADOR\OneDrive\Área de Trabalho\SMG\robo de mensagens\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F289448-621E-46E4-9E5A-7DC159510FAD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02002530-9FE3-4E91-ACF6-DBCEED536222}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>felipe</t>
   </si>
@@ -39,19 +39,39 @@
   </si>
   <si>
     <t xml:space="preserve">marcus </t>
+  </si>
+  <si>
+    <t>Nome</t>
+  </si>
+  <si>
+    <t>Número</t>
+  </si>
+  <si>
+    <t>Mensagem</t>
+  </si>
+  <si>
+    <t>5513974248436</t>
+  </si>
+  <si>
+    <t>5513996227988</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -74,8 +94,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -356,36 +380,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>5513974248436</v>
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>5513996227988</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>